<commit_message>
#23.1 Edit All Model
</commit_message>
<xml_diff>
--- a/src/public/design DB Backend HoiDanIT.xlsx
+++ b/src/public/design DB Backend HoiDanIT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FullStack\src\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECF4306F-6E21-4809-999C-C0CEE94D43B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380A59A1-CB67-4A14-9DFB-CF5037AC1C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1217,7 +1216,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>